<commit_message>
Chason: add automatic generate ID function
</commit_message>
<xml_diff>
--- a/Backend/dashboardApp/DawnEventsCopy.xlsx
+++ b/Backend/dashboardApp/DawnEventsCopy.xlsx
@@ -263,7 +263,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1111,7 +1111,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="5" t="s">
         <v>60</v>
       </c>
@@ -1136,7 +1136,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="5">
         <v>45423</v>
       </c>
@@ -1161,7 +1161,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="5">
         <v>45302</v>
       </c>
@@ -1186,7 +1186,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="5">
         <v>45302</v>
       </c>

</xml_diff>